<commit_message>
Update distribution table definition
</commit_message>
<xml_diff>
--- a/app/config/tables/distributions/forms/distributions/distributions.xlsx
+++ b/app/config/tables/distributions/forms/distributions/distributions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22680" windowHeight="16215" tabRatio="989" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="22680" windowHeight="8330" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,17 @@
     <sheet name="properties" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>type</t>
   </si>
@@ -156,6 +151,15 @@
   </si>
   <si>
     <t>We are not giving volunteers the ability to create or edit distributions</t>
+  </si>
+  <si>
+    <t>location_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>location_name</t>
   </si>
 </sst>
 </file>
@@ -638,19 +642,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="47.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -666,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -674,7 +678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -682,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -690,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -698,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -706,19 +710,35 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="11" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -736,13 +756,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="46.625" customWidth="1"/>
+    <col min="2" max="2" width="46.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -753,7 +773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -762,7 +782,7 @@
       </c>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -771,7 +791,7 @@
       </c>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -780,7 +800,7 @@
       </c>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -789,7 +809,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -812,9 +832,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -838,7 +858,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -856,20 +876,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="29.75" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
@@ -886,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>25</v>
       </c>
@@ -903,7 +923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -920,7 +940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>32</v>
       </c>

</xml_diff>